<commit_message>
don't know how git ignore works but dont need these
</commit_message>
<xml_diff>
--- a/data/UFM_estimate.xlsx
+++ b/data/UFM_estimate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliapop/Desktop/SanJuansPaleo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992B3680-D976-004D-88FC-D075D2C2F510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA8D5A9-D1E1-CF46-9829-33574928361A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="820" windowWidth="16340" windowHeight="17440" xr2:uid="{0F63D018-841E-AB48-BD25-D978856E9A3C}"/>
+    <workbookView xWindow="4720" yWindow="820" windowWidth="24420" windowHeight="17440" xr2:uid="{0F63D018-841E-AB48-BD25-D978856E9A3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -514,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA3D3F4-4B06-3449-82A5-C5B9FB122FE8}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>